<commit_message>
Nov 15, 16 - object select, config design
</commit_message>
<xml_diff>
--- a/Copy of GAPIT interface.xlsx
+++ b/Copy of GAPIT interface.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="38320" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Single" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="213">
   <si>
     <t>Y</t>
   </si>
@@ -507,9 +507,6 @@
   </si>
   <si>
     <t>EMMA parameter</t>
-  </si>
-  <si>
-    <t>maximum number ofloops in FarmCPU</t>
   </si>
   <si>
     <t>FarmCPU parameter</t>
@@ -661,6 +658,18 @@
   </si>
   <si>
     <t>kinship.algorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMMA parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maximum number ofloops in FarmCPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FarmCPU parameter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -674,6 +683,7 @@
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1175,9 +1185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61:B97"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1217,7 +1227,7 @@
         <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H1" t="s">
         <v>144</v>
@@ -1670,17 +1680,17 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15">
         <f t="shared" ref="C15:C23" si="5">LEN(D15)</f>
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
@@ -1690,7 +1700,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
@@ -1703,17 +1713,17 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
@@ -1723,7 +1733,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="3"/>
@@ -1756,7 +1766,7 @@
         <v>139</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="3"/>
@@ -1888,7 +1898,7 @@
         <v>141</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="H21" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1921,7 +1931,7 @@
         <v>141</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H22" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1954,7 +1964,7 @@
         <v>141</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>160</v>
+        <v>211</v>
       </c>
       <c r="H23" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1988,7 +1998,7 @@
         <v>92</v>
       </c>
       <c r="G24" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H24" s="46" t="str">
         <f t="shared" si="3"/>
@@ -2022,7 +2032,7 @@
         <v>92</v>
       </c>
       <c r="G25" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H25" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2056,7 +2066,7 @@
         <v>92</v>
       </c>
       <c r="G26" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H26" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2090,7 +2100,7 @@
         <v>92</v>
       </c>
       <c r="G27" s="48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H27" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2124,7 +2134,7 @@
         <v>92</v>
       </c>
       <c r="G28" s="48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H28" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2158,7 +2168,7 @@
         <v>92</v>
       </c>
       <c r="G29" s="48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H29" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2192,7 +2202,7 @@
         <v>92</v>
       </c>
       <c r="G30" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H30" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2226,7 +2236,7 @@
         <v>92</v>
       </c>
       <c r="G31" s="48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H31" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2260,7 +2270,7 @@
         <v>92</v>
       </c>
       <c r="G32" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H32" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2294,7 +2304,7 @@
         <v>92</v>
       </c>
       <c r="G33" s="48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H33" s="49" t="str">
         <f t="shared" si="3"/>
@@ -2328,7 +2338,7 @@
         <v>92</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H34" s="49" t="str">
         <f t="shared" ref="H34:H65" si="9">D34&amp;"="&amp;B34&amp;","&amp;" #"&amp;G34</f>
@@ -2362,7 +2372,7 @@
         <v>92</v>
       </c>
       <c r="G35" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H35" s="52" t="str">
         <f t="shared" si="9"/>
@@ -2396,7 +2406,7 @@
         <v>93</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H36" s="9" t="str">
         <f t="shared" si="9"/>
@@ -2430,7 +2440,7 @@
         <v>93</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H37" s="9" t="str">
         <f t="shared" si="9"/>
@@ -2464,7 +2474,7 @@
         <v>93</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H38" s="9" t="str">
         <f t="shared" si="9"/>
@@ -2477,10 +2487,10 @@
     </row>
     <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C39" s="21">
         <f t="shared" si="6"/>
@@ -2498,7 +2508,7 @@
         <v>94</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H39" s="21" t="str">
         <f t="shared" si="9"/>
@@ -2514,7 +2524,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C40" s="18">
         <f t="shared" si="6"/>
@@ -2532,7 +2542,7 @@
         <v>94</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H40" s="18" t="str">
         <f t="shared" si="9"/>
@@ -2548,7 +2558,7 @@
         <v>44</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C41" s="25">
         <f t="shared" si="6"/>
@@ -2566,7 +2576,7 @@
         <v>94</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H41" s="25" t="str">
         <f t="shared" si="9"/>
@@ -2600,7 +2610,7 @@
         <v>48</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H42" s="13" t="str">
         <f t="shared" si="9"/>
@@ -2634,7 +2644,7 @@
         <v>48</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H43" s="13" t="str">
         <f t="shared" si="9"/>
@@ -2668,7 +2678,7 @@
         <v>48</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H44" s="13" t="str">
         <f t="shared" si="9"/>
@@ -2684,7 +2694,7 @@
         <v>40</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="37">
         <f>LEN(D45)</f>
@@ -2701,7 +2711,7 @@
         <v>95</v>
       </c>
       <c r="G45" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H45" s="37" t="str">
         <f t="shared" si="9"/>
@@ -2717,7 +2727,7 @@
         <v>54</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C46" s="40">
         <f>LEN(A46)</f>
@@ -2735,7 +2745,7 @@
         <v>95</v>
       </c>
       <c r="G46" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H46" s="40" t="str">
         <f t="shared" si="9"/>
@@ -2751,7 +2761,7 @@
         <v>55</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C47" s="40">
         <f>LEN(A47)</f>
@@ -2769,7 +2779,7 @@
         <v>95</v>
       </c>
       <c r="G47" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H47" s="40" t="str">
         <f t="shared" si="9"/>
@@ -2785,7 +2795,7 @@
         <v>57</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C48" s="40">
         <f>LEN(A48)</f>
@@ -2803,7 +2813,7 @@
         <v>95</v>
       </c>
       <c r="G48" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H48" s="40" t="str">
         <f t="shared" si="9"/>
@@ -2819,7 +2829,7 @@
         <v>56</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C49" s="43">
         <f>LEN(A49)</f>
@@ -2837,7 +2847,7 @@
         <v>95</v>
       </c>
       <c r="G49" s="42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H49" s="43" t="str">
         <f t="shared" si="9"/>
@@ -2871,7 +2881,7 @@
         <v>118</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H50" s="15" t="str">
         <f t="shared" si="9"/>
@@ -2904,7 +2914,7 @@
         <v>119</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H51" s="9" t="str">
         <f t="shared" si="9"/>
@@ -2937,7 +2947,7 @@
         <v>119</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H52" s="9" t="str">
         <f t="shared" si="9"/>
@@ -2970,7 +2980,7 @@
         <v>119</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H53" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3003,7 +3013,7 @@
         <v>119</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H54" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3036,7 +3046,7 @@
         <v>119</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H55" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3069,7 +3079,7 @@
         <v>119</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H56" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3103,7 +3113,7 @@
         <v>119</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H57" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3137,7 +3147,7 @@
         <v>119</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H58" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3153,7 +3163,7 @@
         <v>65</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C59" s="9">
         <f>LEN(D59)</f>
@@ -3170,7 +3180,7 @@
         <v>119</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H59" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3203,7 +3213,7 @@
         <v>119</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H60" s="9" t="str">
         <f t="shared" si="9"/>
@@ -3304,7 +3314,7 @@
         <v>73</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H63" s="13" t="str">
         <f t="shared" si="9"/>
@@ -3337,7 +3347,7 @@
         <v>73</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H64" s="13" t="str">
         <f t="shared" si="9"/>
@@ -3371,7 +3381,7 @@
         <v>73</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H65" s="13" t="str">
         <f t="shared" si="9"/>
@@ -3387,7 +3397,7 @@
         <v>69</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C66" s="13">
         <f>LEN(A66)</f>
@@ -3405,7 +3415,7 @@
         <v>73</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H66" s="13" t="str">
         <f t="shared" ref="H66:H97" si="13">D66&amp;"="&amp;B66&amp;","&amp;" #"&amp;G66</f>
@@ -3439,7 +3449,7 @@
         <v>73</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H67" s="13" t="str">
         <f t="shared" si="13"/>
@@ -3473,7 +3483,7 @@
         <v>73</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H68" s="13" t="str">
         <f t="shared" si="13"/>
@@ -3507,7 +3517,7 @@
         <v>73</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H69" s="13" t="str">
         <f t="shared" si="13"/>
@@ -3540,7 +3550,7 @@
         <v>96</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H70" s="28" t="str">
         <f t="shared" si="13"/>
@@ -3573,7 +3583,7 @@
         <v>96</v>
       </c>
       <c r="G71" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H71" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3607,7 +3617,7 @@
         <v>96</v>
       </c>
       <c r="G72" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H72" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3623,7 +3633,7 @@
         <v>78</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C73" s="31">
         <f t="shared" si="15"/>
@@ -3641,7 +3651,7 @@
         <v>96</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H73" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3675,7 +3685,7 @@
         <v>96</v>
       </c>
       <c r="G74" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H74" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3709,7 +3719,7 @@
         <v>96</v>
       </c>
       <c r="G75" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H75" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3725,7 +3735,7 @@
         <v>81</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C76" s="31">
         <f t="shared" si="15"/>
@@ -3743,7 +3753,7 @@
         <v>96</v>
       </c>
       <c r="G76" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H76" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3777,7 +3787,7 @@
         <v>96</v>
       </c>
       <c r="G77" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H77" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3811,7 +3821,7 @@
         <v>96</v>
       </c>
       <c r="G78" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H78" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3845,7 +3855,7 @@
         <v>96</v>
       </c>
       <c r="G79" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H79" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3861,7 +3871,7 @@
         <v>85</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C80" s="31">
         <f t="shared" si="15"/>
@@ -3879,7 +3889,7 @@
         <v>96</v>
       </c>
       <c r="G80" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H80" s="31" t="str">
         <f t="shared" si="13"/>
@@ -3913,7 +3923,7 @@
         <v>96</v>
       </c>
       <c r="G81" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H81" s="34" t="str">
         <f t="shared" si="13"/>
@@ -3946,7 +3956,7 @@
         <v>140</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H82" s="7" t="str">
         <f t="shared" si="13"/>
@@ -3979,7 +3989,7 @@
         <v>140</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H83" s="7" t="str">
         <f t="shared" si="13"/>
@@ -3992,17 +4002,17 @@
     </row>
     <row r="84" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A84" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C84" s="7">
         <f t="shared" si="17"/>
         <v>19</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E84" s="7">
         <f t="shared" si="12"/>
@@ -4012,7 +4022,7 @@
         <v>140</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H84" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4025,17 +4035,17 @@
     </row>
     <row r="85" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A85" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="C85" s="7">
         <f t="shared" si="17"/>
         <v>14</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E85" s="7">
         <f t="shared" si="12"/>
@@ -4045,7 +4055,7 @@
         <v>140</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H85" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4078,7 +4088,7 @@
         <v>140</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H86" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4111,7 +4121,7 @@
         <v>140</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H87" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4144,7 +4154,7 @@
         <v>140</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H88" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4177,7 +4187,7 @@
         <v>140</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H89" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4210,7 +4220,7 @@
         <v>140</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H90" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4243,7 +4253,7 @@
         <v>140</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H91" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4276,7 +4286,7 @@
         <v>140</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H92" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4309,7 +4319,7 @@
         <v>140</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H93" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4342,7 +4352,7 @@
         <v>140</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H94" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4375,7 +4385,7 @@
         <v>140</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H95" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4408,7 +4418,7 @@
         <v>140</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H96" s="7" t="str">
         <f t="shared" si="13"/>
@@ -4441,7 +4451,7 @@
         <v>140</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H97" s="7" t="str">
         <f t="shared" si="13"/>

</xml_diff>